<commit_message>
export images, some other cleanup
</commit_message>
<xml_diff>
--- a/analysis/runsBottomFirst/bottomFirst.xlsx
+++ b/analysis/runsBottomFirst/bottomFirst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Documents\baseballstats\analysis\runsBottomFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FAABCF-ECB9-4905-93D6-77456757B65F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E254523C-E34D-4037-A949-D670A64B9378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="2903" windowWidth="19845" windowHeight="10792" xr2:uid="{CD636656-7C08-48FA-A201-503286E17550}"/>
+    <workbookView xWindow="4455" yWindow="2415" windowWidth="19845" windowHeight="12225" xr2:uid="{CD636656-7C08-48FA-A201-503286E17550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>"expected" runs in bottom 1st</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>8-15</t>
+  </si>
+  <si>
+    <t>batters</t>
   </si>
 </sst>
 </file>
@@ -140,6 +143,61 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runs in bottom of 1st by pitches thrown in top of 1st</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -150,15 +208,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>runs in bottom 1st</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>actual runs</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -236,20 +286,12 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>"expected" runs in bottom 1st</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>expected runs</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -337,6 +379,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pitches thrown in top 1st</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -402,6 +499,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>runs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -445,6 +597,599 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runs in bottom of 1st by batters faced in top of 1st</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>actual runs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.59564439999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60255429999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59614986000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61734133999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61930470000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59660179999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60576920000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A3D7-499E-B8DD-64D46304DD9D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>expected runs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$20:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5493613516037662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A3D7-499E-B8DD-64D46304DD9D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="661241144"/>
+        <c:axId val="661243112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="661241144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Batters faced in top</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> 1st</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="661243112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="661243112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>runs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="661241144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -490,6 +1235,43 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1045,20 +1827,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>440530</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>207166</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>478630</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>328611</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1078,6 +2376,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>216692</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1074491-3F33-4555-AE8F-FC2BD601C7AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1383,10 +2717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CDE4D6-36D6-43ED-B955-C82A73A2EE80}">
-  <dimension ref="A1:XFD5"/>
+  <dimension ref="A1:XFD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1473,6 +2807,84 @@
       </c>
       <c r="XFD5" s="1"/>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>0.59564439999999996</v>
+      </c>
+      <c r="C21">
+        <v>0.60255429999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.59614986000000003</v>
+      </c>
+      <c r="E21">
+        <v>0.61734133999999996</v>
+      </c>
+      <c r="F21">
+        <v>0.61930470000000004</v>
+      </c>
+      <c r="G21">
+        <v>0.59660179999999996</v>
+      </c>
+      <c r="H21">
+        <v>0.60576920000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.5493613516037662</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>